<commit_message>
update to adapt new batch of data
</commit_message>
<xml_diff>
--- a/2-Config-Files/cds_config/UI-database mappings.xlsx
+++ b/2-Config-Files/cds_config/UI-database mappings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangf6/Documents/cds_v1.2/2-Config-Files/cds_config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15309670-4A4D-7946-B54F-66597DE1151E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3646A9C-4FA3-BE4A-BB8E-E2E72055F0B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7600" yWindow="500" windowWidth="34460" windowHeight="26520" activeTab="1" xr2:uid="{0BC66A93-5BEB-764C-8BB9-E5211772CAA1}"/>
+    <workbookView xWindow="3940" yWindow="500" windowWidth="34460" windowHeight="19100" activeTab="1" xr2:uid="{0BC66A93-5BEB-764C-8BB9-E5211772CAA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="61">
   <si>
     <t>Data page</t>
   </si>
@@ -225,6 +225,24 @@
   </si>
   <si>
     <t>file.experimental_strategy_and_data_subtypes</t>
+  </si>
+  <si>
+    <t>study.study_access</t>
+  </si>
+  <si>
+    <t>study</t>
+  </si>
+  <si>
+    <t>study_access</t>
+  </si>
+  <si>
+    <t>file.file_access</t>
+  </si>
+  <si>
+    <t>file</t>
+  </si>
+  <si>
+    <t>file_access</t>
   </si>
 </sst>
 </file>
@@ -1153,10 +1171,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F09E50E9-33B3-FE43-9963-D716D4024E8E}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="165" zoomScaleNormal="165" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1357,6 +1375,28 @@
         <v>study_name</v>
       </c>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update to adapt April released data
</commit_message>
<xml_diff>
--- a/2-Config-Files/cds_config/UI-database mappings.xlsx
+++ b/2-Config-Files/cds_config/UI-database mappings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangf6/Documents/cds_v1.2/2-Config-Files/cds_config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3646A9C-4FA3-BE4A-BB8E-E2E72055F0B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459E64DD-9441-044D-B034-5AE129F4A783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3940" yWindow="500" windowWidth="34460" windowHeight="19100" activeTab="1" xr2:uid="{0BC66A93-5BEB-764C-8BB9-E5211772CAA1}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="65">
   <si>
     <t>Data page</t>
   </si>
@@ -243,6 +243,18 @@
   </si>
   <si>
     <t>file_access</t>
+  </si>
+  <si>
+    <t>file.file_size</t>
+  </si>
+  <si>
+    <t>file_size</t>
+  </si>
+  <si>
+    <t>file.md5sum</t>
+  </si>
+  <si>
+    <t>md5sum</t>
   </si>
 </sst>
 </file>
@@ -1171,7 +1183,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F09E50E9-33B3-FE43-9963-D716D4024E8E}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="165" zoomScaleNormal="165" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
@@ -1397,6 +1409,28 @@
         <v>60</v>
       </c>
     </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>